<commit_message>
after haunting mars #3
</commit_message>
<xml_diff>
--- a/haunting_mars/miners.xlsx
+++ b/haunting_mars/miners.xlsx
@@ -1,16 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dare/Documents/personal/rpg/posthuman/haunting_mars/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD4947E-B58D-D145-869B-940C7E5EA07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="28620" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="28620" windowHeight="16980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,12 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dare Talvitie</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -40,20 +57,56 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">4 = expert
-3 = miner
-2 = has relevant skills
-1 = has 1 relevant skill
-0 = wtf
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">3 = miner
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">2 = has relevant skills
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1 = has 1 relevant skill
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">0 = wtf
 </t>
         </r>
       </text>
@@ -63,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="167">
   <si>
     <t>Name</t>
   </si>
@@ -106,6 +159,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -179,6 +233,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -524,13 +579,73 @@
   </si>
   <si>
     <t>Kwame Larbi</t>
+  </si>
+  <si>
+    <t>Milana Alfiya</t>
+  </si>
+  <si>
+    <t>robotics sales assistant</t>
+  </si>
+  <si>
+    <t>cyborg pride</t>
+  </si>
+  <si>
+    <t>vacuum pod</t>
+  </si>
+  <si>
+    <t>vacuum  pod</t>
+  </si>
+  <si>
+    <t>shaken</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>hard shell</t>
+  </si>
+  <si>
+    <t>Rina Aly</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>gym instructor</t>
+  </si>
+  <si>
+    <t>Thaddeus Brown</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>H&amp;S Engineer</t>
+  </si>
+  <si>
+    <t>hardworking</t>
+  </si>
+  <si>
+    <t>so pretty</t>
+  </si>
+  <si>
+    <t>cycle power</t>
+  </si>
+  <si>
+    <t>yellow-turqoisee</t>
+  </si>
+  <si>
+    <t>pants+headband</t>
+  </si>
+  <si>
+    <t>patterned</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -552,11 +667,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -579,6 +696,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -609,20 +746,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -631,6 +769,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -955,1147 +1101,1315 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="2" style="3" customWidth="1"/>
-    <col min="3" max="3" width="6" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" style="3" customWidth="1"/>
-    <col min="5" max="6" width="4.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="4" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="3"/>
-    <col min="10" max="11" width="3.6640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="3" style="3" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="3"/>
-    <col min="14" max="14" width="13.6640625" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="2" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="6" width="4.33203125" customWidth="1"/>
+    <col min="7" max="7" width="4" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="10" max="11" width="3.6640625" customWidth="1"/>
+    <col min="12" max="12" width="3" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="30">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2">
         <v>2100</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2">
         <v>33</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2">
         <f>2147-C2-E2</f>
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2">
         <v>2</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2">
         <v>1</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" t="s">
         <v>127</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" t="s">
         <v>55</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" t="s">
         <v>62</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" t="s">
         <v>66</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>2107</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>26</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
         <f t="shared" ref="F3:F18" si="0">2147-C3-E3</f>
         <v>14</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="3">
-        <v>0</v>
-      </c>
-      <c r="K3" s="3">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" t="s">
         <v>127</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" t="s">
         <v>59</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" t="s">
         <v>79</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" t="s">
         <v>66</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="8" customFormat="1">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>2093</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>40</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="8">
         <v>4</v>
       </c>
-      <c r="L4" s="9"/>
-      <c r="N4" s="8" t="s">
+      <c r="L4" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="N4" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="P4" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>2118</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
         <v>15</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="3">
-        <v>0</v>
-      </c>
-      <c r="K5" s="3">
-        <v>0</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
         <v>127</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" t="s">
         <v>62</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" t="s">
         <v>83</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>2078</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>54</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
         <v>15</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" t="s">
         <v>86</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6">
         <v>1</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6">
         <v>3</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" t="s">
         <v>127</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" t="s">
         <v>137</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" t="s">
         <v>75</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" t="s">
         <v>76</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>2077</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="2">
         <v>70</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" t="s">
         <v>20</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7">
         <v>1</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7">
         <v>3</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" t="s">
         <v>127</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" t="s">
         <v>64</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" t="s">
         <v>67</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="8" customFormat="1">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>2081</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>66</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="7">
         <v>4</v>
       </c>
-      <c r="N8" s="8" t="s">
+      <c r="L8" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="N8" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="O8" s="8" t="s">
+      <c r="O8" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="P8" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>1</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>2099</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
         <v>33</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3" t="s">
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
         <v>127</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M9" t="s">
         <v>115</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="N9" t="s">
         <v>79</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="O9" t="s">
         <v>116</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="P9" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>1</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10">
         <v>2111</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10">
         <v>22</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s">
         <v>87</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="3">
-        <v>0</v>
-      </c>
-      <c r="K10" s="3">
-        <v>0</v>
-      </c>
-      <c r="L10" s="3" t="s">
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
         <v>127</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="M10" t="s">
         <v>60</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="N10" t="s">
         <v>73</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="O10" t="s">
         <v>74</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="P10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>1</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11">
         <v>2091</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11">
         <v>43</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" t="s">
         <v>87</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" t="s">
         <v>4</v>
       </c>
-      <c r="J11" s="3">
-        <v>0</v>
-      </c>
-      <c r="K11" s="3">
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
         <v>2</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" t="s">
         <v>127</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="M11" t="s">
         <v>57</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="N11" t="s">
         <v>68</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="O11" t="s">
         <v>95</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="P11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>2</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <v>2114</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12">
         <v>19</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" t="s">
         <v>88</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" t="s">
         <v>4</v>
       </c>
-      <c r="J12" s="3">
-        <v>0</v>
-      </c>
-      <c r="K12" s="3">
-        <v>0</v>
-      </c>
-      <c r="L12" s="3" t="s">
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
         <v>127</v>
       </c>
-      <c r="M12" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="N12" s="3" t="s">
+      <c r="M12" t="s">
+        <v>166</v>
+      </c>
+      <c r="N12" t="s">
         <v>80</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="O12" t="s">
         <v>81</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="P12" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>2</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13">
         <v>2078</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="2">
         <v>67</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" t="s">
         <v>36</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J13" s="3">
-        <v>0</v>
-      </c>
-      <c r="K13" s="3">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
         <v>2</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L13" t="s">
         <v>127</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="M13" t="s">
         <v>126</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="N13" t="s">
         <v>62</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="O13" t="s">
         <v>72</v>
       </c>
-      <c r="P13" s="3" t="s">
+      <c r="P13" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>2</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14">
         <v>2085</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="2">
         <v>58</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" t="s">
         <v>40</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="3">
-        <v>0</v>
-      </c>
-      <c r="K14" s="3">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
         <v>3</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="L14" t="s">
         <v>127</v>
       </c>
-      <c r="M14" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="N14" s="3" t="s">
+      <c r="M14" t="s">
+        <v>164</v>
+      </c>
+      <c r="N14" t="s">
         <v>69</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="O14" t="s">
         <v>67</v>
       </c>
-      <c r="P14" s="3" t="s">
+      <c r="P14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>2</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15">
         <v>2115</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15">
         <v>18</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" t="s">
         <v>86</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" t="s">
         <v>4</v>
       </c>
-      <c r="J15" s="3">
-        <v>0</v>
-      </c>
-      <c r="K15" s="3">
-        <v>0</v>
-      </c>
-      <c r="L15" s="3" t="s">
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
         <v>127</v>
       </c>
-      <c r="M15" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="N15" s="3" t="s">
+      <c r="M15" t="s">
+        <v>165</v>
+      </c>
+      <c r="N15" t="s">
         <v>63</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="O15" t="s">
         <v>81</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="P15" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>2</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16">
         <v>2115</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" t="s">
         <v>45</v>
       </c>
       <c r="E16" s="2">
         <v>32</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" t="s">
         <v>46</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="3">
-        <v>0</v>
-      </c>
-      <c r="K16" s="3">
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
         <v>1</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="L16" t="s">
         <v>127</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="M16" t="s">
         <v>135</v>
       </c>
-      <c r="N16" s="3" t="s">
+      <c r="N16" t="s">
         <v>70</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="O16" t="s">
         <v>71</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="P16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>2</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17">
         <v>2108</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17">
         <v>25</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" t="s">
         <v>86</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" t="s">
         <v>50</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" t="s">
         <v>4</v>
       </c>
-      <c r="J17" s="3">
-        <v>0</v>
-      </c>
-      <c r="K17" s="3">
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
         <v>2</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="L17" t="s">
         <v>127</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="M17" t="s">
         <v>126</v>
       </c>
-      <c r="N17" s="3" t="s">
+      <c r="N17" t="s">
         <v>80</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="O17" t="s">
         <v>66</v>
       </c>
-      <c r="P17" s="3" t="s">
+      <c r="P17" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>2</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18">
         <v>2097</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18">
         <v>36</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" t="s">
         <v>53</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="I18" t="s">
         <v>4</v>
       </c>
-      <c r="J18" s="3">
-        <v>0</v>
-      </c>
-      <c r="K18" s="3">
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
         <v>1</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="L18" t="s">
         <v>127</v>
       </c>
-      <c r="M18" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="N18" s="3" t="s">
+      <c r="M18" t="s">
+        <v>150</v>
+      </c>
+      <c r="N18" t="s">
         <v>82</v>
       </c>
-      <c r="O18" s="3" t="s">
+      <c r="O18" t="s">
         <v>83</v>
       </c>
-      <c r="P18" s="3" t="s">
+      <c r="P18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>2</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19">
         <v>2114</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" t="s">
         <v>138</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19">
         <v>22</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19">
         <v>11</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" t="s">
         <v>16</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J19" s="3">
-        <v>0</v>
-      </c>
-      <c r="K19" s="3">
-        <v>0</v>
-      </c>
-      <c r="L19" s="3" t="s">
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
         <v>127</v>
       </c>
-      <c r="M19" s="3" t="s">
+      <c r="M19" t="s">
         <v>126</v>
       </c>
-      <c r="N19" s="3" t="s">
+      <c r="N19" t="s">
         <v>139</v>
       </c>
-      <c r="O19" s="3" t="s">
+      <c r="O19" t="s">
         <v>96</v>
       </c>
-      <c r="P19" s="3" t="s">
+      <c r="P19" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>2</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20">
         <v>2108</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20">
         <v>36</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20">
         <v>3</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" t="s">
         <v>92</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20">
         <v>3</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20">
         <v>2</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="L20" t="s">
         <v>127</v>
       </c>
-      <c r="O20" s="3" t="s">
+      <c r="M20" t="s">
+        <v>150</v>
+      </c>
+      <c r="O20" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>2</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21">
         <v>2111</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" t="s">
         <v>97</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21">
         <v>35</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21">
         <v>2</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" t="s">
         <v>99</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21">
         <v>3</v>
       </c>
-      <c r="K21" s="3">
-        <v>0</v>
-      </c>
-      <c r="L21" s="3" t="s">
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
         <v>127</v>
       </c>
-      <c r="O21" s="3" t="s">
+      <c r="M21" t="s">
+        <v>143</v>
+      </c>
+      <c r="O21" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>2</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22">
         <v>2116</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" t="s">
         <v>104</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22">
         <v>21</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22">
         <v>8</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" t="s">
         <v>100</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22">
         <v>3</v>
       </c>
-      <c r="K22" s="3">
-        <v>0</v>
-      </c>
-      <c r="L22" s="3" t="s">
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22" t="s">
         <v>127</v>
       </c>
-      <c r="O22" s="3" t="s">
+      <c r="M22" t="s">
+        <v>151</v>
+      </c>
+      <c r="N22" t="s">
+        <v>152</v>
+      </c>
+      <c r="O22" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>2</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23">
         <v>2126</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" t="s">
         <v>105</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23">
         <v>7</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23">
         <v>14</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" t="s">
         <v>88</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" t="s">
         <v>101</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" t="s">
         <v>4</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23">
         <v>3</v>
       </c>
-      <c r="K23" s="3">
-        <v>0</v>
-      </c>
-      <c r="L23" s="3" t="s">
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
         <v>127</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="M23" t="s">
         <v>143</v>
       </c>
-      <c r="O23" s="3" t="s">
+      <c r="O23" t="s">
         <v>102</v>
       </c>
-      <c r="P23" s="3" t="s">
+      <c r="P23" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B24" s="11">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>2090</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24">
+        <v>43</v>
+      </c>
+      <c r="F24">
+        <v>14</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H24" t="s">
+        <v>148</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>153</v>
+      </c>
+      <c r="M24" t="s">
+        <v>126</v>
+      </c>
+      <c r="N24" t="s">
+        <v>80</v>
+      </c>
+      <c r="O24" t="s">
+        <v>149</v>
+      </c>
+      <c r="P24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B25" s="4">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>2105</v>
+      </c>
+      <c r="D25" t="s">
+        <v>156</v>
+      </c>
+      <c r="E25">
+        <v>28</v>
+      </c>
+      <c r="F25">
+        <v>14</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H25" t="s">
+        <v>157</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25" t="s">
+        <v>153</v>
+      </c>
+      <c r="M25" t="s">
+        <v>126</v>
+      </c>
+      <c r="N25" t="s">
+        <v>80</v>
+      </c>
+      <c r="O25" t="s">
+        <v>71</v>
+      </c>
+      <c r="P25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B26" s="4">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>2107</v>
+      </c>
+      <c r="D26" t="s">
+        <v>159</v>
+      </c>
+      <c r="E26">
+        <v>26</v>
+      </c>
+      <c r="F26">
+        <v>14</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" t="s">
+        <v>160</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="M26" t="s">
+        <v>126</v>
+      </c>
+      <c r="N26" t="s">
+        <v>80</v>
+      </c>
+      <c r="O26" t="s">
+        <v>161</v>
+      </c>
+      <c r="P26" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
after Haunting Mars 5
</commit_message>
<xml_diff>
--- a/haunting_mars/miners.xlsx
+++ b/haunting_mars/miners.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11116"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dare/Documents/personal/rpg/posthuman/haunting_mars/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD4947E-B58D-D145-869B-940C7E5EA07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC82877D-7EA0-D04A-A9B0-29C8D7DD23E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2400" windowWidth="28620" windowHeight="16980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="168">
   <si>
     <t>Name</t>
   </si>
@@ -639,6 +639,9 @@
   </si>
   <si>
     <t>patterned</t>
+  </si>
+  <si>
+    <t>Recent</t>
   </si>
 </sst>
 </file>
@@ -1102,11 +1105,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1121,9 +1124,10 @@
     <col min="10" max="11" width="3.6640625" customWidth="1"/>
     <col min="12" max="12" width="3" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" customWidth="1"/>
+    <col min="15" max="15" width="7.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1167,13 +1171,16 @@
         <v>61</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1217,14 +1224,17 @@
       <c r="N2" t="s">
         <v>62</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
         <v>66</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1268,14 +1278,17 @@
       <c r="N3" t="s">
         <v>79</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3">
+        <v>-1</v>
+      </c>
+      <c r="P3" t="s">
         <v>66</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -1316,14 +1329,14 @@
       <c r="N4" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="P4" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="Q4" s="7" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>107</v>
       </c>
@@ -1367,14 +1380,17 @@
       <c r="N5" t="s">
         <v>62</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
         <v>83</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1417,14 +1433,17 @@
       <c r="N6" t="s">
         <v>75</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6">
+        <v>-1</v>
+      </c>
+      <c r="P6" t="s">
         <v>76</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>108</v>
       </c>
@@ -1468,14 +1487,17 @@
       <c r="N7" t="s">
         <v>64</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
         <v>67</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
@@ -1516,14 +1538,14 @@
       <c r="N8" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="P8" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="Q8" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>122</v>
       </c>
@@ -1567,14 +1589,17 @@
       <c r="N9" t="s">
         <v>79</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
         <v>116</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>121</v>
       </c>
@@ -1618,14 +1643,17 @@
       <c r="N10" t="s">
         <v>73</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10">
+        <v>-2</v>
+      </c>
+      <c r="P10" t="s">
         <v>74</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>106</v>
       </c>
@@ -1669,14 +1697,17 @@
       <c r="N11" t="s">
         <v>68</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
         <v>95</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1720,14 +1751,17 @@
       <c r="N12" t="s">
         <v>80</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12">
+        <v>-2</v>
+      </c>
+      <c r="P12" t="s">
         <v>81</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>129</v>
       </c>
@@ -1771,14 +1805,17 @@
       <c r="N13" t="s">
         <v>62</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13" t="s">
         <v>72</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -1822,14 +1859,17 @@
       <c r="N14" t="s">
         <v>69</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
         <v>67</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>132</v>
       </c>
@@ -1873,14 +1913,17 @@
       <c r="N15" t="s">
         <v>63</v>
       </c>
-      <c r="O15" t="s">
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
         <v>81</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -1924,14 +1967,17 @@
       <c r="N16" t="s">
         <v>70</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
         <v>71</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
@@ -1975,14 +2021,17 @@
       <c r="N17" t="s">
         <v>80</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
         <v>66</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
@@ -2026,14 +2075,17 @@
       <c r="N18" t="s">
         <v>82</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O18">
+        <v>-1</v>
+      </c>
+      <c r="P18" t="s">
         <v>83</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>141</v>
       </c>
@@ -2076,14 +2128,17 @@
       <c r="N19" t="s">
         <v>139</v>
       </c>
-      <c r="O19" t="s">
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19" t="s">
         <v>96</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>89</v>
       </c>
@@ -2123,11 +2178,11 @@
       <c r="M20" t="s">
         <v>150</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>145</v>
       </c>
@@ -2167,11 +2222,11 @@
       <c r="M21" t="s">
         <v>143</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>98</v>
       </c>
@@ -2214,11 +2269,11 @@
       <c r="N22" t="s">
         <v>152</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>146</v>
       </c>
@@ -2258,14 +2313,14 @@
       <c r="M23" t="s">
         <v>143</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>102</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>147</v>
       </c>
@@ -2308,14 +2363,14 @@
       <c r="N24" t="s">
         <v>80</v>
       </c>
-      <c r="O24" t="s">
-        <v>149</v>
-      </c>
       <c r="P24" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>155</v>
       </c>
@@ -2358,14 +2413,14 @@
       <c r="N25" t="s">
         <v>80</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>71</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>158</v>
       </c>
@@ -2399,16 +2454,19 @@
       <c r="K26">
         <v>1</v>
       </c>
+      <c r="L26" t="s">
+        <v>153</v>
+      </c>
       <c r="M26" t="s">
         <v>126</v>
       </c>
       <c r="N26" t="s">
         <v>80</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>161</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>163</v>
       </c>
     </row>

</xml_diff>